<commit_message>
fixed name auto populating
</commit_message>
<xml_diff>
--- a/public/Catalog Worksheet/InputOptions.xlsx
+++ b/public/Catalog Worksheet/InputOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjbischo\Dropbox (ASU)\Projects\ShinyDataEntry\public\Catalog Worksheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9B904E-F720-4F79-8F91-494A8CEE138F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888FDCFF-0EA2-443C-99FF-1EE28E844B03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{A8A7240E-B734-4FC6-8922-4656482CB74A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15396" xr2:uid="{A8A7240E-B734-4FC6-8922-4656482CB74A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="114">
   <si>
     <t>numeric</t>
   </si>
@@ -370,6 +361,12 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>user</t>
   </si>
 </sst>
 </file>
@@ -721,26 +718,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527FEE92-9FDA-4DCE-8B2F-08DAE0774CC2}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -748,7 +745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -756,12 +753,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -793,7 +790,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -804,7 +801,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -815,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -829,7 +826,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -840,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -851,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -862,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -873,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -884,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -901,7 +898,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -915,7 +912,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -929,7 +926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -940,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -951,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -968,7 +965,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -982,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -996,7 +993,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1010,7 +1007,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1024,7 +1021,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1038,7 +1035,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1052,7 +1049,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1066,7 +1063,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1080,7 +1077,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1094,7 +1091,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1111,7 +1108,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1128,7 +1125,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1136,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1150,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -1164,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1184,7 +1181,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1204,7 +1201,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1218,7 +1215,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1232,7 +1229,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1246,7 +1243,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -1260,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1280,7 +1277,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1300,7 +1297,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1320,7 +1317,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1363,7 +1360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1386,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1409,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1429,7 +1426,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -1449,7 +1446,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -1466,7 +1463,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1474,10 +1471,10 @@
         <v>97</v>
       </c>
       <c r="D51" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1489,6 +1486,17 @@
       </c>
       <c r="H52" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>